<commit_message>
added TestNG params for day 4 challenge
</commit_message>
<xml_diff>
--- a/src/main/java/com/kalopap/guru99/Resources/TestData.xlsx
+++ b/src/main/java/com/kalopap/guru99/Resources/TestData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Selenium\EndToEndPOCs\Guru99poc7d\src\main\java\com\kalopap\guru99\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D65ED07D-C9F9-4730-8B66-F1684759DC98}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B5DDC988-A000-44C4-AB0D-49C76A539B82}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{B22ED2AA-20C6-4FDE-AB55-3823A910AC17}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16830" windowHeight="2520" xr2:uid="{B22ED2AA-20C6-4FDE-AB55-3823A910AC17}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -43,6 +39,21 @@
   </si>
   <si>
     <t>pupEgaj</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Invalid 1</t>
+  </si>
+  <si>
+    <t>Invalid 2</t>
+  </si>
+  <si>
+    <t>Invalid 3</t>
+  </si>
+  <si>
+    <t>Valid 1</t>
   </si>
 </sst>
 </file>
@@ -394,51 +405,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2D4D79-9EE1-486E-8FF2-6D26A903F4F2}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
testdata from DataProvider and Screenshot code added
</commit_message>
<xml_diff>
--- a/src/main/java/com/kalopap/guru99/Resources/TestData.xlsx
+++ b/src/main/java/com/kalopap/guru99/Resources/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B5DDC988-A000-44C4-AB0D-49C76A539B82}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{25F4FED2-1CA4-41C8-9D93-D39FE6066624}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16830" windowHeight="2520" xr2:uid="{B22ED2AA-20C6-4FDE-AB55-3823A910AC17}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="6015" xr2:uid="{B22ED2AA-20C6-4FDE-AB55-3823A910AC17}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>